<commit_message>
reformat how data output
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bliss-Moreau Lab\Desktop\PlayingWithAOIs\TEAS-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony Santistevan\Dropbox\Projects\inProgress\psychopy\TEAS\bml\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>smile.jpg</t>
   </si>
@@ -45,12 +45,21 @@
   </si>
   <si>
     <t>Picture2</t>
+  </si>
+  <si>
+    <t>ProbeLocation</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>frown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -380,8 +389,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -391,8 +403,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -402,60 +417,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tracks mouse coords during trial
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>smile.jpg</t>
   </si>
@@ -32,9 +32,6 @@
     <t>frown.jpg</t>
   </si>
   <si>
-    <t>Locations</t>
-  </si>
-  <si>
     <t>[-0.35, 0]</t>
   </si>
   <si>
@@ -47,13 +44,16 @@
     <t>Picture2</t>
   </si>
   <si>
-    <t>ProbeLocation</t>
-  </si>
-  <si>
     <t>smile</t>
   </si>
   <si>
     <t>frown</t>
+  </si>
+  <si>
+    <t>probeCoords</t>
+  </si>
+  <si>
+    <t>stimOverProbe</t>
   </si>
 </sst>
 </file>
@@ -371,26 +371,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -401,10 +401,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -418,7 +418,35 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>